<commit_message>
Rettelser til hurtig upload
Generelt rettelse af placering og tilføjelse af enkelte filer
</commit_message>
<xml_diff>
--- a/Excel/Lister.xlsx
+++ b/Excel/Lister.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Områder" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Forespørgsel_fra_groenreg" localSheetId="1" hidden="1">Elementer!$A$1:$G$128</definedName>
+    <definedName name="Forespørgsel_fra_groenreg" localSheetId="1" hidden="1">Elementer!$A$1:$G$129</definedName>
     <definedName name="Forespørgsel_fra_groenreg" localSheetId="2" hidden="1">Områder!$A$1:$D$250</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1784" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="777">
   <si>
     <t>h_element_kode</t>
   </si>
@@ -2377,6 +2377,12 @@
   </si>
   <si>
     <t>ANA-02-02</t>
+  </si>
+  <si>
+    <t>BE-06-05</t>
+  </si>
+  <si>
+    <t>Støbt gummi</t>
   </si>
 </sst>
 </file>
@@ -2446,7 +2452,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="53">
     <dxf>
       <font>
         <strike val="0"/>
@@ -2460,6 +2466,36 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2476,18 +2512,34 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2504,6 +2556,27 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2518,6 +2591,36 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -2530,6 +2633,291 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <border>
@@ -2681,7 +3069,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Tabeltypografi 1" pivot="0" count="1">
-      <tableStyleElement type="wholeTable" dxfId="17"/>
+      <tableStyleElement type="wholeTable" dxfId="52"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -2728,8 +3116,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel_Forespørgsel_fra_groenreg" displayName="Tabel_Forespørgsel_fra_groenreg" ref="A1:M128" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:M128"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel_Forespørgsel_fra_groenreg" displayName="Tabel_Forespørgsel_fra_groenreg" ref="A1:M129" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:M129"/>
   <tableColumns count="13">
     <tableColumn id="1" uniqueName="1" name="h_element_kode" queryTableFieldId="1"/>
     <tableColumn id="2" uniqueName="2" name="hovedelement_tekst" queryTableFieldId="2"/>
@@ -2738,19 +3126,19 @@
     <tableColumn id="5" uniqueName="5" name="u_element_kode" queryTableFieldId="5"/>
     <tableColumn id="6" uniqueName="6" name="underlement_tekst" queryTableFieldId="6"/>
     <tableColumn id="7" uniqueName="7" name="objekt_type" queryTableFieldId="7"/>
-    <tableColumn id="8" uniqueName="8" name="Hovedelement" queryTableFieldId="8" dataDxfId="5">
+    <tableColumn id="8" uniqueName="8" name="Hovedelement" queryTableFieldId="8" dataDxfId="18">
       <calculatedColumnFormula>IF(H1=B1,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B1,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" uniqueName="9" name=" " queryTableFieldId="9" dataDxfId="4">
+    <tableColumn id="9" uniqueName="9" name=" " queryTableFieldId="9" dataDxfId="15">
       <calculatedColumnFormula>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D1,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" uniqueName="10" name="Element" queryTableFieldId="10" dataDxfId="3">
+    <tableColumn id="10" uniqueName="10" name="Element" queryTableFieldId="10" dataDxfId="11">
       <calculatedColumnFormula>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D1,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" uniqueName="11" name="  " queryTableFieldId="11" dataDxfId="2">
+    <tableColumn id="11" uniqueName="11" name="  " queryTableFieldId="11" dataDxfId="8">
       <calculatedColumnFormula>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F1,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" uniqueName="12" name="Underelement" queryTableFieldId="12" dataDxfId="1">
+    <tableColumn id="12" uniqueName="12" name="Underelement" queryTableFieldId="12" dataDxfId="4">
       <calculatedColumnFormula>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F1,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" uniqueName="13" name="Type" queryTableFieldId="13" dataDxfId="0">
@@ -3115,7 +3503,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M128"/>
+  <dimension ref="A1:M129"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="H89" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J118" sqref="J118"/>
@@ -6753,49 +7141,49 @@
     </row>
     <row r="78" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>229</v>
+        <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>230</v>
+        <v>18</v>
       </c>
       <c r="C78" t="s">
-        <v>231</v>
+        <v>63</v>
       </c>
       <c r="D78" t="s">
-        <v>230</v>
+        <v>64</v>
       </c>
       <c r="E78" t="s">
-        <v>232</v>
+        <v>775</v>
       </c>
       <c r="F78" t="s">
-        <v>230</v>
+        <v>776</v>
       </c>
       <c r="G78" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H78" s="1" t="str">
         <f>IF(H77=B77,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B77,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
-        <v>Terrænudstyr</v>
+        <v/>
       </c>
       <c r="I78" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D77,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>00</v>
+        <v/>
       </c>
       <c r="J78" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D77,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Terrænudstyr</v>
+        <v/>
       </c>
       <c r="K78" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F77,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>00</v>
+        <v>05</v>
       </c>
       <c r="L78" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F77,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Terrænudstyr</v>
+        <v>Støbt gummi</v>
       </c>
       <c r="M78" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>FLP</v>
+        <v>F</v>
       </c>
     </row>
     <row r="79" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -6806,39 +7194,39 @@
         <v>230</v>
       </c>
       <c r="C79" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D79" t="s">
-        <v>288</v>
+        <v>230</v>
       </c>
       <c r="E79" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F79" t="s">
-        <v>288</v>
+        <v>230</v>
       </c>
       <c r="G79" t="s">
         <v>344</v>
       </c>
       <c r="H79" s="1" t="str">
         <f>IF(H78=B78,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B78,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
-        <v>UD</v>
+        <v>Terrænudstyr</v>
       </c>
       <c r="I79" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D78,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>01</v>
+        <v>00</v>
       </c>
       <c r="J79" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D78,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Andet terrænudstyr</v>
+        <v>Terrænudstyr</v>
       </c>
       <c r="K79" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F78,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>01</v>
+        <v>00</v>
       </c>
       <c r="L79" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F78,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Andet terrænudstyr</v>
+        <v>Terrænudstyr</v>
       </c>
       <c r="M79" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -6859,37 +7247,37 @@
         <v>288</v>
       </c>
       <c r="E80" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F80" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G80" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H80" s="1" t="str">
         <f>IF(H79=B79,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B79,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
-        <v/>
+        <v>UD</v>
       </c>
       <c r="I80" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D79,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v/>
+        <v>01</v>
       </c>
       <c r="J80" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D79,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v/>
+        <v>Andet terrænudstyr</v>
       </c>
       <c r="K80" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F79,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L80" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F79,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Skilt</v>
+        <v>Andet terrænudstyr</v>
       </c>
       <c r="M80" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>P</v>
+        <v>FLP</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -6906,10 +7294,10 @@
         <v>288</v>
       </c>
       <c r="E81" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F81" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G81" t="s">
         <v>345</v>
@@ -6928,11 +7316,11 @@
       </c>
       <c r="K81" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F80,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="L81" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F80,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Trafikbom</v>
+        <v>Skilt</v>
       </c>
       <c r="M81" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -6953,13 +7341,13 @@
         <v>288</v>
       </c>
       <c r="E82" t="s">
-        <v>750</v>
+        <v>239</v>
       </c>
       <c r="F82" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G82" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="H82" s="1" t="str">
         <f>IF(H81=B81,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B81,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
@@ -6975,15 +7363,15 @@
       </c>
       <c r="K82" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F81,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>04</v>
+        <v>03</v>
       </c>
       <c r="L82" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F81,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Pullert</v>
+        <v>Trafikbom</v>
       </c>
       <c r="M82" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>LP</v>
+        <v>P</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -7000,10 +7388,10 @@
         <v>288</v>
       </c>
       <c r="E83" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="F83" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G83" t="s">
         <v>349</v>
@@ -7022,11 +7410,11 @@
       </c>
       <c r="K83" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F82,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L83" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F82,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Cykelstativ</v>
+        <v>Pullert</v>
       </c>
       <c r="M83" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -7047,13 +7435,13 @@
         <v>288</v>
       </c>
       <c r="E84" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="F84" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G84" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="H84" s="1" t="str">
         <f>IF(H83=B83,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B83,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
@@ -7069,15 +7457,15 @@
       </c>
       <c r="K84" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F83,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>06</v>
+        <v>05</v>
       </c>
       <c r="L84" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F83,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Parklys</v>
+        <v>Cykelstativ</v>
       </c>
       <c r="M84" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>P</v>
+        <v>LP</v>
       </c>
     </row>
     <row r="85" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -7094,10 +7482,10 @@
         <v>288</v>
       </c>
       <c r="E85" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="F85" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G85" t="s">
         <v>345</v>
@@ -7116,11 +7504,11 @@
       </c>
       <c r="K85" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F84,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>07</v>
+        <v>06</v>
       </c>
       <c r="L85" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F84,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Banelys</v>
+        <v>Parklys</v>
       </c>
       <c r="M85" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -7141,13 +7529,13 @@
         <v>288</v>
       </c>
       <c r="E86" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F86" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G86" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H86" s="1" t="str">
         <f>IF(H85=B85,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B85,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
@@ -7163,15 +7551,15 @@
       </c>
       <c r="K86" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F85,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>08</v>
+        <v>07</v>
       </c>
       <c r="L86" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F85,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Tagrende</v>
+        <v>Banelys</v>
       </c>
       <c r="M86" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>L</v>
+        <v>P</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -7188,13 +7576,13 @@
         <v>288</v>
       </c>
       <c r="E87" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F87" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G87" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H87" s="1" t="str">
         <f>IF(H86=B86,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B86,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
@@ -7210,15 +7598,15 @@
       </c>
       <c r="K87" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F86,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>09</v>
+        <v>08</v>
       </c>
       <c r="L87" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F86,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Lyskasse</v>
+        <v>Tagrende</v>
       </c>
       <c r="M87" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>P</v>
+        <v>L</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -7235,10 +7623,10 @@
         <v>288</v>
       </c>
       <c r="E88" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F88" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G88" t="s">
         <v>345</v>
@@ -7257,11 +7645,11 @@
       </c>
       <c r="K88" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F87,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>10</v>
+        <v>09</v>
       </c>
       <c r="L88" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F87,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Faskine</v>
+        <v>Lyskasse</v>
       </c>
       <c r="M88" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -7282,10 +7670,10 @@
         <v>288</v>
       </c>
       <c r="E89" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="F89" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G89" t="s">
         <v>345</v>
@@ -7304,11 +7692,11 @@
       </c>
       <c r="K89" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F88,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L89" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F88,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Affaldscontainer</v>
+        <v>Faskine</v>
       </c>
       <c r="M89" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -7329,10 +7717,10 @@
         <v>288</v>
       </c>
       <c r="E90" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F90" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G90" t="s">
         <v>345</v>
@@ -7351,11 +7739,11 @@
       </c>
       <c r="K90" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F89,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L90" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F89,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Shelterhytte</v>
+        <v>Affaldscontainer</v>
       </c>
       <c r="M90" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -7376,13 +7764,13 @@
         <v>288</v>
       </c>
       <c r="E91" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="F91" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G91" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H91" s="1" t="str">
         <f>IF(H90=B90,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B90,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
@@ -7398,15 +7786,15 @@
       </c>
       <c r="K91" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F90,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L91" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F90,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Træbro</v>
+        <v>Shelterhytte</v>
       </c>
       <c r="M91" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>L</v>
+        <v>P</v>
       </c>
     </row>
     <row r="92" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -7423,13 +7811,13 @@
         <v>288</v>
       </c>
       <c r="E92" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="F92" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G92" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H92" s="1" t="str">
         <f>IF(H91=B91,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B91,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
@@ -7445,15 +7833,15 @@
       </c>
       <c r="K92" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F91,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L92" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F91,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Kampesten</v>
+        <v>Træbro</v>
       </c>
       <c r="M92" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>P</v>
+        <v>L</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -7470,10 +7858,10 @@
         <v>288</v>
       </c>
       <c r="E93" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="F93" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G93" t="s">
         <v>345</v>
@@ -7492,11 +7880,11 @@
       </c>
       <c r="K93" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F92,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L93" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F92,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Flagstang</v>
+        <v>Kampesten</v>
       </c>
       <c r="M93" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -7511,19 +7899,19 @@
         <v>230</v>
       </c>
       <c r="C94" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D94" t="s">
-        <v>234</v>
+        <v>288</v>
       </c>
       <c r="E94" t="s">
-        <v>243</v>
+        <v>761</v>
       </c>
       <c r="F94" t="s">
-        <v>762</v>
+        <v>304</v>
       </c>
       <c r="G94" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="H94" s="1" t="str">
         <f>IF(H93=B93,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B93,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
@@ -7531,23 +7919,23 @@
       </c>
       <c r="I94" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D93,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>02</v>
+        <v/>
       </c>
       <c r="J94" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D93,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Trapper</v>
+        <v/>
       </c>
       <c r="K94" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F93,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>01</v>
+        <v>15</v>
       </c>
       <c r="L94" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F93,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Trappe</v>
+        <v>Flagstang</v>
       </c>
       <c r="M94" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>F</v>
+        <v>P</v>
       </c>
     </row>
     <row r="95" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -7564,10 +7952,10 @@
         <v>234</v>
       </c>
       <c r="E95" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F95" t="s">
-        <v>236</v>
+        <v>762</v>
       </c>
       <c r="G95" t="s">
         <v>343</v>
@@ -7578,19 +7966,19 @@
       </c>
       <c r="I95" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D94,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v/>
+        <v>02</v>
       </c>
       <c r="J95" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D94,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v/>
+        <v>Trapper</v>
       </c>
       <c r="K95" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F94,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L95" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F94,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Betontrappe</v>
+        <v>Trappe</v>
       </c>
       <c r="M95" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -7611,10 +7999,10 @@
         <v>234</v>
       </c>
       <c r="E96" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F96" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G96" t="s">
         <v>343</v>
@@ -7633,11 +8021,11 @@
       </c>
       <c r="K96" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F95,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="L96" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F95,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Naturstenstrappe</v>
+        <v>Betontrappe</v>
       </c>
       <c r="M96" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -7658,10 +8046,10 @@
         <v>234</v>
       </c>
       <c r="E97" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F97" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G97" t="s">
         <v>343</v>
@@ -7680,11 +8068,11 @@
       </c>
       <c r="K97" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F96,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>04</v>
+        <v>03</v>
       </c>
       <c r="L97" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F96,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Trappe - træ/jord</v>
+        <v>Naturstenstrappe</v>
       </c>
       <c r="M97" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -7699,19 +8087,19 @@
         <v>230</v>
       </c>
       <c r="C98" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="D98" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="E98" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F98" t="s">
-        <v>763</v>
+        <v>240</v>
       </c>
       <c r="G98" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H98" s="1" t="str">
         <f>IF(H97=B97,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B97,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
@@ -7719,23 +8107,23 @@
       </c>
       <c r="I98" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D97,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>03</v>
+        <v/>
       </c>
       <c r="J98" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D97,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Terrænmure</v>
+        <v/>
       </c>
       <c r="K98" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F97,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>01</v>
+        <v>04</v>
       </c>
       <c r="L98" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F97,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Terrænmur</v>
+        <v>Trappe - træ/jord</v>
       </c>
       <c r="M98" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>L</v>
+        <v>F</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -7752,10 +8140,10 @@
         <v>242</v>
       </c>
       <c r="E99" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F99" t="s">
-        <v>244</v>
+        <v>763</v>
       </c>
       <c r="G99" t="s">
         <v>346</v>
@@ -7766,19 +8154,19 @@
       </c>
       <c r="I99" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D98,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v/>
+        <v>03</v>
       </c>
       <c r="J99" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D98,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v/>
+        <v>Terrænmure</v>
       </c>
       <c r="K99" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F98,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L99" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F98,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Kampestensmur</v>
+        <v>Terrænmur</v>
       </c>
       <c r="M99" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -7799,10 +8187,10 @@
         <v>242</v>
       </c>
       <c r="E100" t="s">
-        <v>764</v>
+        <v>255</v>
       </c>
       <c r="F100" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G100" t="s">
         <v>346</v>
@@ -7821,11 +8209,11 @@
       </c>
       <c r="K100" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F99,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="L100" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F99,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Betonmur</v>
+        <v>Kampestensmur</v>
       </c>
       <c r="M100" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -7846,10 +8234,10 @@
         <v>242</v>
       </c>
       <c r="E101" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="F101" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G101" t="s">
         <v>346</v>
@@ -7868,11 +8256,11 @@
       </c>
       <c r="K101" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F100,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>04</v>
+        <v>03</v>
       </c>
       <c r="L101" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F100,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Naturstensmur</v>
+        <v>Betonmur</v>
       </c>
       <c r="M101" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -7893,10 +8281,10 @@
         <v>242</v>
       </c>
       <c r="E102" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="F102" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G102" t="s">
         <v>346</v>
@@ -7915,11 +8303,11 @@
       </c>
       <c r="K102" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F101,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L102" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F101,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Træmur</v>
+        <v>Naturstensmur</v>
       </c>
       <c r="M102" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -7934,19 +8322,19 @@
         <v>230</v>
       </c>
       <c r="C103" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D103" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="E103" t="s">
-        <v>259</v>
+        <v>766</v>
       </c>
       <c r="F103" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G103" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H103" s="1" t="str">
         <f>IF(H102=B102,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B102,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
@@ -7954,23 +8342,23 @@
       </c>
       <c r="I103" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D102,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>04</v>
+        <v/>
       </c>
       <c r="J103" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D102,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Bænke</v>
+        <v/>
       </c>
       <c r="K103" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F102,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>01</v>
+        <v>05</v>
       </c>
       <c r="L103" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F102,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Bænk</v>
+        <v>Træmur</v>
       </c>
       <c r="M103" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>P</v>
+        <v>L</v>
       </c>
     </row>
     <row r="104" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -7987,10 +8375,10 @@
         <v>252</v>
       </c>
       <c r="E104" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F104" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G104" t="s">
         <v>345</v>
@@ -8001,19 +8389,19 @@
       </c>
       <c r="I104" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D103,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v/>
+        <v>04</v>
       </c>
       <c r="J104" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D103,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v/>
+        <v>Bænke</v>
       </c>
       <c r="K104" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F103,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L104" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F103,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Bord- og bænkesæt</v>
+        <v>Bænk</v>
       </c>
       <c r="M104" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -8028,19 +8416,19 @@
         <v>230</v>
       </c>
       <c r="C105" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="D105" t="s">
-        <v>767</v>
+        <v>252</v>
       </c>
       <c r="E105" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="F105" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G105" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H105" s="1" t="str">
         <f>IF(H104=B104,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B104,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
@@ -8048,23 +8436,23 @@
       </c>
       <c r="I105" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D104,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>05</v>
+        <v/>
       </c>
       <c r="J105" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D104,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Faste hegn</v>
+        <v/>
       </c>
       <c r="K105" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F104,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="L105" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F104,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Fast hegn</v>
+        <v>Bord- og bænkesæt</v>
       </c>
       <c r="M105" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>L</v>
+        <v>P</v>
       </c>
     </row>
     <row r="106" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -8081,10 +8469,10 @@
         <v>767</v>
       </c>
       <c r="E106" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F106" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G106" t="s">
         <v>346</v>
@@ -8095,19 +8483,19 @@
       </c>
       <c r="I106" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D105,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v/>
+        <v>05</v>
       </c>
       <c r="J106" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D105,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v/>
+        <v>Faste hegn</v>
       </c>
       <c r="K106" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F105,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L106" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F105,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Trådhegn</v>
+        <v>Fast hegn</v>
       </c>
       <c r="M106" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -8128,10 +8516,10 @@
         <v>767</v>
       </c>
       <c r="E107" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F107" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G107" t="s">
         <v>346</v>
@@ -8150,11 +8538,11 @@
       </c>
       <c r="K107" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F106,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="L107" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F106,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Maskinflettet hegn</v>
+        <v>Trådhegn</v>
       </c>
       <c r="M107" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -8175,10 +8563,10 @@
         <v>767</v>
       </c>
       <c r="E108" t="s">
-        <v>741</v>
+        <v>270</v>
       </c>
       <c r="F108" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G108" t="s">
         <v>346</v>
@@ -8197,11 +8585,11 @@
       </c>
       <c r="K108" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F107,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>04</v>
+        <v>03</v>
       </c>
       <c r="L108" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F107,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Træhegn</v>
+        <v>Maskinflettet hegn</v>
       </c>
       <c r="M108" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -8222,10 +8610,10 @@
         <v>767</v>
       </c>
       <c r="E109" t="s">
-        <v>768</v>
+        <v>741</v>
       </c>
       <c r="F109" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G109" t="s">
         <v>346</v>
@@ -8244,11 +8632,11 @@
       </c>
       <c r="K109" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F108,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>05</v>
+        <v>04</v>
       </c>
       <c r="L109" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F108,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Fodhegn</v>
+        <v>Træhegn</v>
       </c>
       <c r="M109" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -8263,19 +8651,19 @@
         <v>230</v>
       </c>
       <c r="C110" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="D110" t="s">
-        <v>266</v>
+        <v>767</v>
       </c>
       <c r="E110" t="s">
-        <v>274</v>
+        <v>768</v>
       </c>
       <c r="F110" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G110" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H110" s="1" t="str">
         <f>IF(H109=B109,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B109,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
@@ -8283,23 +8671,23 @@
       </c>
       <c r="I110" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D109,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>06</v>
+        <v/>
       </c>
       <c r="J110" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D109,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Legeudstyr</v>
+        <v/>
       </c>
       <c r="K110" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F109,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>01</v>
+        <v>05</v>
       </c>
       <c r="L110" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F109,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Legeudstyr</v>
+        <v>Fodhegn</v>
       </c>
       <c r="M110" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>P</v>
+        <v>L</v>
       </c>
     </row>
     <row r="111" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -8316,13 +8704,13 @@
         <v>266</v>
       </c>
       <c r="E111" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F111" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G111" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="H111" s="1" t="str">
         <f>IF(H110=B110,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B110,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
@@ -8330,23 +8718,23 @@
       </c>
       <c r="I111" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D110,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v/>
+        <v>06</v>
       </c>
       <c r="J111" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D110,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v/>
+        <v>Legeudstyr</v>
       </c>
       <c r="K111" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F110,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L111" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F110,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Sandkasse</v>
+        <v>Legeudstyr</v>
       </c>
       <c r="M111" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>F</v>
+        <v>P</v>
       </c>
     </row>
     <row r="112" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -8363,13 +8751,13 @@
         <v>266</v>
       </c>
       <c r="E112" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F112" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G112" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H112" s="1" t="str">
         <f>IF(H111=B111,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B111,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
@@ -8385,15 +8773,15 @@
       </c>
       <c r="K112" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F111,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="L112" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F111,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Kant - faldunderlag</v>
+        <v>Sandkasse</v>
       </c>
       <c r="M112" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>L</v>
+        <v>F</v>
       </c>
     </row>
     <row r="113" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -8410,10 +8798,10 @@
         <v>266</v>
       </c>
       <c r="E113" t="s">
-        <v>769</v>
+        <v>278</v>
       </c>
       <c r="F113" t="s">
-        <v>742</v>
+        <v>271</v>
       </c>
       <c r="G113" t="s">
         <v>346</v>
@@ -8432,11 +8820,11 @@
       </c>
       <c r="K113" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F112,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>04</v>
+        <v>03</v>
       </c>
       <c r="L113" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F112,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Kant - sandkasse</v>
+        <v>Kant - faldunderlag</v>
       </c>
       <c r="M113" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -8451,19 +8839,19 @@
         <v>230</v>
       </c>
       <c r="C114" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="D114" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E114" t="s">
-        <v>282</v>
+        <v>769</v>
       </c>
       <c r="F114" t="s">
-        <v>273</v>
+        <v>742</v>
       </c>
       <c r="G114" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H114" s="1" t="str">
         <f>IF(H113=B113,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B113,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
@@ -8471,23 +8859,23 @@
       </c>
       <c r="I114" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D113,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>07</v>
+        <v/>
       </c>
       <c r="J114" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D113,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Affald</v>
+        <v/>
       </c>
       <c r="K114" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F113,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>01</v>
+        <v>04</v>
       </c>
       <c r="L114" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F113,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Affald</v>
+        <v>Kant - sandkasse</v>
       </c>
       <c r="M114" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>P</v>
+        <v>L</v>
       </c>
     </row>
     <row r="115" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -8504,10 +8892,10 @@
         <v>273</v>
       </c>
       <c r="E115" t="s">
-        <v>770</v>
+        <v>282</v>
       </c>
       <c r="F115" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G115" t="s">
         <v>345</v>
@@ -8518,19 +8906,19 @@
       </c>
       <c r="I115" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D114,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v/>
+        <v>07</v>
       </c>
       <c r="J115" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D114,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v/>
+        <v>Affald</v>
       </c>
       <c r="K115" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F114,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L115" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F114,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Affaldsspand</v>
+        <v>Affald</v>
       </c>
       <c r="M115" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -8551,10 +8939,10 @@
         <v>273</v>
       </c>
       <c r="E116" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F116" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G116" t="s">
         <v>345</v>
@@ -8573,11 +8961,11 @@
       </c>
       <c r="K116" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F115,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="L116" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F115,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Askebæger</v>
+        <v>Affaldsspand</v>
       </c>
       <c r="M116" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -8598,10 +8986,10 @@
         <v>273</v>
       </c>
       <c r="E117" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F117" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G117" t="s">
         <v>345</v>
@@ -8620,11 +9008,11 @@
       </c>
       <c r="K117" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F116,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>04</v>
+        <v>03</v>
       </c>
       <c r="L117" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F116,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Hundeposestativ</v>
+        <v>Askebæger</v>
       </c>
       <c r="M117" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -8639,16 +9027,16 @@
         <v>230</v>
       </c>
       <c r="C118" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D118" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="E118" t="s">
-        <v>285</v>
+        <v>772</v>
       </c>
       <c r="F118" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G118" t="s">
         <v>345</v>
@@ -8659,19 +9047,19 @@
       </c>
       <c r="I118" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D117,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>08</v>
+        <v/>
       </c>
       <c r="J118" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D117,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Busstop</v>
+        <v/>
       </c>
       <c r="K118" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F117,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>01</v>
+        <v>04</v>
       </c>
       <c r="L118" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F117,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Busstop</v>
+        <v>Hundeposestativ</v>
       </c>
       <c r="M118" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -8686,16 +9074,16 @@
         <v>230</v>
       </c>
       <c r="C119" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D119" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E119" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F119" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G119" t="s">
         <v>345</v>
@@ -8706,11 +9094,11 @@
       </c>
       <c r="I119" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D118,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>09</v>
+        <v>08</v>
       </c>
       <c r="J119" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D118,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Fitness</v>
+        <v>Busstop</v>
       </c>
       <c r="K119" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F118,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
@@ -8718,7 +9106,7 @@
       </c>
       <c r="L119" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F118,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Fitness</v>
+        <v>Busstop</v>
       </c>
       <c r="M119" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -8739,10 +9127,10 @@
         <v>284</v>
       </c>
       <c r="E120" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F120" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G120" t="s">
         <v>345</v>
@@ -8753,19 +9141,19 @@
       </c>
       <c r="I120" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D119,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v/>
+        <v>09</v>
       </c>
       <c r="J120" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D119,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v/>
+        <v>Fitness</v>
       </c>
       <c r="K120" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F119,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L120" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F119,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Fast sportsudstyr</v>
+        <v>Fitness</v>
       </c>
       <c r="M120" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -8774,49 +9162,49 @@
     </row>
     <row r="121" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>3</v>
+        <v>229</v>
       </c>
       <c r="B121" t="s">
-        <v>4</v>
+        <v>230</v>
       </c>
       <c r="C121" t="s">
-        <v>5</v>
+        <v>287</v>
       </c>
       <c r="D121" t="s">
-        <v>4</v>
+        <v>284</v>
       </c>
       <c r="E121" t="s">
-        <v>6</v>
+        <v>291</v>
       </c>
       <c r="F121" t="s">
-        <v>4</v>
+        <v>286</v>
       </c>
       <c r="G121" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="H121" s="1" t="str">
         <f>IF(H120=B120,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B120,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
-        <v>Anden anvendelse</v>
+        <v/>
       </c>
       <c r="I121" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D120,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>01</v>
+        <v/>
       </c>
       <c r="J121" s="1" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D120,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Anden anvendelse</v>
+        <v/>
       </c>
       <c r="K121" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F120,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="L121" s="2" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F120,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Anden anvendelse</v>
+        <v>Fast sportsudstyr</v>
       </c>
       <c r="M121" s="2" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>FLP</v>
+        <v>P</v>
       </c>
     </row>
     <row r="122" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -8827,31 +9215,31 @@
         <v>4</v>
       </c>
       <c r="C122" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D122" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E122" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F122" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G122" t="s">
         <v>344</v>
       </c>
       <c r="H122" s="5" t="str">
         <f>IF(H121=B121,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B121,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
-        <v>ANA</v>
+        <v>Anden anvendelse</v>
       </c>
       <c r="I122" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D121,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="J122" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D121,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Udenfor drift og pleje</v>
+        <v>Anden anvendelse</v>
       </c>
       <c r="K122" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F121,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
@@ -8859,7 +9247,7 @@
       </c>
       <c r="L122" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F121,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Udenfor drift og pleje</v>
+        <v>Anden anvendelse</v>
       </c>
       <c r="M122" s="5" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -8880,37 +9268,37 @@
         <v>8</v>
       </c>
       <c r="E123" t="s">
-        <v>774</v>
+        <v>9</v>
       </c>
       <c r="F123" t="s">
-        <v>93</v>
+        <v>8</v>
       </c>
       <c r="G123" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="H123" s="5" t="str">
         <f>IF(H122=B122,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B122,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
-        <v/>
+        <v>ANA</v>
       </c>
       <c r="I123" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D122,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v/>
+        <v>02</v>
       </c>
       <c r="J123" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D122,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v/>
+        <v>Udenfor drift og pleje</v>
       </c>
       <c r="K123" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F122,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="L123" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F122,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Urtehave</v>
+        <v>Udenfor drift og pleje</v>
       </c>
       <c r="M123" s="5" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>F</v>
+        <v>FLP</v>
       </c>
     </row>
     <row r="124" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -8921,16 +9309,16 @@
         <v>4</v>
       </c>
       <c r="C124" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D124" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E124" t="s">
-        <v>12</v>
+        <v>774</v>
       </c>
       <c r="F124" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="G124" t="s">
         <v>343</v>
@@ -8941,19 +9329,19 @@
       </c>
       <c r="I124" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D123,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>03</v>
+        <v/>
       </c>
       <c r="J124" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D123,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Private haver</v>
+        <v/>
       </c>
       <c r="K124" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F123,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
-        <v>01</v>
+        <v>02</v>
       </c>
       <c r="L124" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F123,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Privat have</v>
+        <v>Urtehave</v>
       </c>
       <c r="M124" s="5" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -8968,19 +9356,19 @@
         <v>4</v>
       </c>
       <c r="C125" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D125" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E125" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F125" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G125" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H125" s="5" t="str">
         <f>IF(H124=B124,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B124,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
@@ -8988,11 +9376,11 @@
       </c>
       <c r="I125" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D124,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>04</v>
+        <v>03</v>
       </c>
       <c r="J125" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D124,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Kantsten</v>
+        <v>Private haver</v>
       </c>
       <c r="K125" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F124,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
@@ -9000,46 +9388,46 @@
       </c>
       <c r="L125" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F124,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Kantsten</v>
+        <v>Privat have</v>
       </c>
       <c r="M125" s="5" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>L</v>
+        <v>F</v>
       </c>
     </row>
     <row r="126" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>178</v>
+        <v>3</v>
       </c>
       <c r="B126" t="s">
-        <v>179</v>
+        <v>4</v>
       </c>
       <c r="C126" t="s">
-        <v>180</v>
+        <v>14</v>
       </c>
       <c r="D126" t="s">
-        <v>181</v>
+        <v>15</v>
       </c>
       <c r="E126" t="s">
-        <v>182</v>
+        <v>16</v>
       </c>
       <c r="F126" t="s">
-        <v>181</v>
+        <v>15</v>
       </c>
       <c r="G126" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H126" s="5" t="str">
         <f>IF(H125=B125,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B125,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
-        <v>Renhold</v>
+        <v/>
       </c>
       <c r="I126" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D125,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>01</v>
+        <v>04</v>
       </c>
       <c r="J126" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D125,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Bypræg</v>
+        <v>Kantsten</v>
       </c>
       <c r="K126" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F125,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
@@ -9047,11 +9435,11 @@
       </c>
       <c r="L126" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F125,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Bypræg</v>
+        <v>Kantsten</v>
       </c>
       <c r="M126" s="5" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
-        <v>P</v>
+        <v>L</v>
       </c>
     </row>
     <row r="127" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -9062,31 +9450,31 @@
         <v>179</v>
       </c>
       <c r="C127" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D127" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E127" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F127" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G127" t="s">
         <v>345</v>
       </c>
       <c r="H127" s="5" t="str">
         <f>IF(H126=B126,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B126,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
-        <v>REN</v>
+        <v>Renhold</v>
       </c>
       <c r="I127" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D126,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>02</v>
+        <v>01</v>
       </c>
       <c r="J127" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D126,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Parkpræg</v>
+        <v>Bypræg</v>
       </c>
       <c r="K127" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F126,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
@@ -9094,7 +9482,7 @@
       </c>
       <c r="L127" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F126,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Parkpræg</v>
+        <v>Bypræg</v>
       </c>
       <c r="M127" s="5" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
@@ -9109,31 +9497,31 @@
         <v>179</v>
       </c>
       <c r="C128" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D128" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E128" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F128" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G128" t="s">
         <v>345</v>
       </c>
       <c r="H128" s="5" t="str">
         <f>IF(H127=B127,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B127,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
-        <v/>
+        <v>REN</v>
       </c>
       <c r="I128" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D127,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
-        <v>03</v>
+        <v>02</v>
       </c>
       <c r="J128" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D127,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
-        <v>Naturpræg</v>
+        <v>Parkpræg</v>
       </c>
       <c r="K128" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F127,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
@@ -9141,59 +9529,140 @@
       </c>
       <c r="L128" s="5" t="str">
         <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F127,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
-        <v>Naturpræg</v>
+        <v>Parkpræg</v>
       </c>
       <c r="M128" s="5" t="str">
         <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
         <v>P</v>
       </c>
     </row>
+    <row r="129" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>178</v>
+      </c>
+      <c r="B129" t="s">
+        <v>179</v>
+      </c>
+      <c r="C129" t="s">
+        <v>186</v>
+      </c>
+      <c r="D129" t="s">
+        <v>187</v>
+      </c>
+      <c r="E129" t="s">
+        <v>188</v>
+      </c>
+      <c r="F129" t="s">
+        <v>187</v>
+      </c>
+      <c r="G129" t="s">
+        <v>345</v>
+      </c>
+      <c r="H129" s="5" t="str">
+        <f>IF(H128=B128,Tabel_Forespørgsel_fra_groenreg[[#This Row],[h_element_kode]],IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]]&lt;&gt;B128,Tabel_Forespørgsel_fra_groenreg[[#This Row],[hovedelement_tekst]],""))</f>
+        <v/>
+      </c>
+      <c r="I129" s="5" t="str">
+        <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D128,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_kode]],2),"")</f>
+        <v>03</v>
+      </c>
+      <c r="J129" s="5" t="str">
+        <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]]&lt;&gt;D128,Tabel_Forespørgsel_fra_groenreg[[#This Row],[element_tekst]],"")</f>
+        <v>Naturpræg</v>
+      </c>
+      <c r="K129" s="5" t="str">
+        <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F128,RIGHT(Tabel_Forespørgsel_fra_groenreg[[#This Row],[u_element_kode]],2),"")</f>
+        <v>01</v>
+      </c>
+      <c r="L129" s="5" t="str">
+        <f>IF(Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]]&lt;&gt;F128,Tabel_Forespørgsel_fra_groenreg[[#This Row],[underlement_tekst]],"")</f>
+        <v>Naturpræg</v>
+      </c>
+      <c r="M129" s="5" t="str">
+        <f>Tabel_Forespørgsel_fra_groenreg[[#This Row],[objekt_type]]</f>
+        <v>P</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:H128">
-    <cfRule type="expression" dxfId="16" priority="10">
+  <conditionalFormatting sqref="H2:H129">
+    <cfRule type="expression" dxfId="51" priority="10">
       <formula>H2=B2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="11">
+    <cfRule type="expression" dxfId="50" priority="11">
       <formula>OR(H2=A2,H2="")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I128">
-    <cfRule type="expression" dxfId="14" priority="9">
+  <conditionalFormatting sqref="I2:I127 I129">
+    <cfRule type="expression" dxfId="49" priority="9">
       <formula>D2&lt;&gt;D1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K128">
-    <cfRule type="expression" dxfId="13" priority="6">
+  <conditionalFormatting sqref="K2:K127 K129">
+    <cfRule type="expression" dxfId="48" priority="6">
       <formula>D2&lt;&gt;D1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:M128">
-    <cfRule type="expression" dxfId="12" priority="1">
+  <conditionalFormatting sqref="H2:M129">
+    <cfRule type="expression" dxfId="47" priority="1">
       <formula>A3=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M128">
-    <cfRule type="expression" dxfId="11" priority="2">
+  <conditionalFormatting sqref="M2:M127 M129">
+    <cfRule type="expression" dxfId="46" priority="2">
       <formula>I2=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="45" priority="3">
       <formula>D2&lt;&gt;D1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L128">
-    <cfRule type="expression" dxfId="9" priority="4">
+  <conditionalFormatting sqref="L2:L127 L129">
+    <cfRule type="expression" dxfId="44" priority="4">
       <formula>D2&lt;&gt;D1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="43" priority="5">
       <formula>J2=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J128">
-    <cfRule type="expression" dxfId="7" priority="7">
+  <conditionalFormatting sqref="J2:J127 J129">
+    <cfRule type="expression" dxfId="42" priority="7">
       <formula>J2=""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="41" priority="8">
       <formula>D2&lt;&gt;D1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I128">
+    <cfRule type="expression" dxfId="40" priority="17">
+      <formula>D128&lt;&gt;D126</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K128">
+    <cfRule type="expression" dxfId="39" priority="19">
+      <formula>D128&lt;&gt;D126</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M128">
+    <cfRule type="expression" dxfId="38" priority="24">
+      <formula>I128=""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="25">
+      <formula>D128&lt;&gt;D126</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L128">
+    <cfRule type="expression" dxfId="36" priority="28">
+      <formula>D128&lt;&gt;D126</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="29">
+      <formula>J128=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J128">
+    <cfRule type="expression" dxfId="34" priority="32">
+      <formula>J128=""</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="33">
+      <formula>D128&lt;&gt;D126</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9214,10 +9683,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="62.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>